<commit_message>
Se agregan pruebas del programador de turnos del sprint 39 y 40
</commit_message>
<xml_diff>
--- a/QA-MP-Plantilla.xlsx
+++ b/QA-MP-Plantilla.xlsx
@@ -5,20 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\QA\Mapas de prueba\Tecnoquimicas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\QA\EXC\InspeccionVehicular\Mapas de prueba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB273AF-A911-4077-9289-360AC171D8EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D2CB06-FB97-4AE1-AF3C-40DA8214E206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{61885951-8E7D-4612-9932-062ECDC3B8B8}"/>
+    <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{61885951-8E7D-4612-9932-062ECDC3B8B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Resultados de pruebas" sheetId="9" r:id="rId1"/>
     <sheet name="Matriz EP" sheetId="1" r:id="rId2"/>
+    <sheet name="Evidencias" sheetId="10" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="130" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="24">
   <si>
     <t>Nro.</t>
   </si>
@@ -59,9 +60,6 @@
   </si>
   <si>
     <t xml:space="preserve">Evidencia </t>
-  </si>
-  <si>
-    <t>NOMBRE DEL PROYECTO</t>
   </si>
   <si>
     <t>Funcional</t>
@@ -96,12 +94,21 @@
   <si>
     <t>HU:</t>
   </si>
+  <si>
+    <t>Evidencia</t>
+  </si>
+  <si>
+    <t>Inpección Vehicular</t>
+  </si>
+  <si>
+    <t>INSPECCIÓN VEHICULAR</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,14 +159,6 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1" tint="0.14999847407452621"/>
       <name val="Calibri"/>
@@ -173,8 +172,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1" tint="0.14999847407452621"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,8 +217,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -343,12 +361,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -368,9 +415,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -382,18 +426,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -407,55 +439,150 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="19">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="10"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -486,76 +613,6 @@
           <bgColor theme="0" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -669,15 +726,50 @@
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color theme="10"/>
+        <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -906,13 +998,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -922,6 +1007,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -996,7 +1088,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[QA-MP-05032024.xlsx]Resultados de pruebas!TablaDinámica31</c:name>
+    <c:name>[QA-MP-Plantilla.xlsx]Resultados de pruebas!TablaDinámica31</c:name>
     <c:fmtId val="3"/>
   </c:pivotSource>
   <c:chart>
@@ -1060,6 +1152,20 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -1093,6 +1199,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-619B-467B-90BB-156EDCAE1331}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -1273,7 +1384,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[QA-MP-05032024.xlsx]Resultados de pruebas!TablaDinámica32</c:name>
+    <c:name>[QA-MP-Plantilla.xlsx]Resultados de pruebas!TablaDinámica32</c:name>
     <c:fmtId val="5"/>
   </c:pivotSource>
   <c:chart>
@@ -1337,6 +1448,20 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -1370,6 +1495,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-DBDA-4D30-9462-E58C46D23348}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -1550,7 +1680,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[QA-MP-05032024.xlsx]Resultados de pruebas!TablaDinámica33</c:name>
+    <c:name>[QA-MP-Plantilla.xlsx]Resultados de pruebas!TablaDinámica33</c:name>
     <c:fmtId val="9"/>
   </c:pivotSource>
   <c:chart>
@@ -1672,6 +1802,20 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -1705,6 +1849,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-5667-4604-8799-DFEA1691690C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -3716,6 +3865,111 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>257175</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89ABDE30-DF4C-4A3F-88D9-8EEDDD6D8930}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr preferRelativeResize="0">
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="238125" y="0"/>
+          <a:ext cx="1019175" cy="485775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>257175</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEC9A3BE-7800-4DDF-8F8F-7BE2BC0B31FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr preferRelativeResize="0">
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="238125" y="0"/>
+          <a:ext cx="1019175" cy="485775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Administrador" refreshedDate="45356.581343981481" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="8" xr:uid="{0D3E433C-791B-4F33-BB5F-9721734836B3}">
   <cacheSource type="worksheet">
@@ -3894,69 +4148,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3A9A497D-0BB6-4034-85A2-64223ED76E77}" name="TablaDinámica33" cacheId="130" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
-  <location ref="A21:B23" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="12">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" showAll="0" sortType="ascending">
-      <items count="2">
-        <item sd="0" x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="9"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Cuenta de Ciclo 3" fld="9" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="9" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{891AABAC-BBBC-4034-8F1E-40BC41AD6F8C}" name="TablaDinámica32" cacheId="130" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{891AABAC-BBBC-4034-8F1E-40BC41AD6F8C}" name="TablaDinámica32" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
   <location ref="A11:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField showAll="0"/>
@@ -3996,12 +4188,24 @@
   <dataFields count="1">
     <dataField name="Cuenta de Ciclo 2" fld="8" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="1">
+  <chartFormats count="2">
     <chartFormat chart="5" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="2"/>
           </reference>
         </references>
       </pivotArea>
@@ -4019,8 +4223,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5BAF725B-D6FF-41E9-9F80-CD463A01DC4E}" name="TablaDinámica31" cacheId="130" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5BAF725B-D6FF-41E9-9F80-CD463A01DC4E}" name="TablaDinámica31" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
   <location ref="A1:B3" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField showAll="0"/>
@@ -4059,11 +4263,97 @@
   <dataFields count="1">
     <dataField name="Cuenta de Ciclo 1" fld="7" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="1">
+  <chartFormats count="2">
     <chartFormat chart="3" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="7" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3A9A497D-0BB6-4034-85A2-64223ED76E77}" name="TablaDinámica33" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
+  <location ref="A21:B23" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="12">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0" sortType="ascending">
+      <items count="2">
+        <item sd="0" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="9"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Cuenta de Ciclo 3" fld="9" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="2">
+    <chartFormat chart="9" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="9" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="9" count="1" selected="0">
             <x v="0"/>
           </reference>
         </references>
@@ -4083,7 +4373,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B1315E74-8D95-4857-90D5-BAEA9EA0A8AD}" name="Tabla5" displayName="Tabla5" ref="B5:M13" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="16" tableBorderDxfId="17" totalsRowBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B1315E74-8D95-4857-90D5-BAEA9EA0A8AD}" name="Tabla5" displayName="Tabla5" ref="B5:M13" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="B5:M13" xr:uid="{B1315E74-8D95-4857-90D5-BAEA9EA0A8AD}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{244A078E-4A46-403E-9A73-EF9D61D60E35}" name="Nro." dataDxfId="14"/>
@@ -4092,12 +4382,14 @@
     <tableColumn id="5" xr3:uid="{67FD9933-1702-4F9A-9178-ED2E7120E3A3}" name="Actividad" dataDxfId="11"/>
     <tableColumn id="7" xr3:uid="{D9DBEE41-B33E-4356-ABAC-56BB5AD33DDA}" name="Dado que" dataDxfId="10"/>
     <tableColumn id="9" xr3:uid="{16369E4B-47E8-4DD9-915A-0F97EBBBED11}" name="Entonces" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{2AB5B15B-1419-408F-BD18-5B5C4BB123FD}" name="Evidencia " dataDxfId="8" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="11" xr3:uid="{2AE4B6D4-966D-47AF-B6A0-1B91D27EE0C2}" name="Ciclo 1" dataDxfId="7"/>
-    <tableColumn id="15" xr3:uid="{C3D5C7FD-622A-40FA-828F-E3F2BF44ADE2}" name="Ciclo 2" dataDxfId="4"/>
-    <tableColumn id="16" xr3:uid="{11BFC6A6-81DE-4299-81B8-ACB7C83EFE82}" name="Ciclo 3" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{665865D4-79FD-48D9-9884-73E6CB75DCDC}" name="Observaciones" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{95C3BFB9-5AE9-4234-996A-372035075F8A}" name="Casos de prueba" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{2AB5B15B-1419-408F-BD18-5B5C4BB123FD}" name="Evidencia " dataDxfId="0" dataCellStyle="Hipervínculo">
+      <calculatedColumnFormula>HYPERLINK("#'Evidencias'!B4", "Evidencia")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{2AE4B6D4-966D-47AF-B6A0-1B91D27EE0C2}" name="Ciclo 1" dataDxfId="8"/>
+    <tableColumn id="15" xr3:uid="{C3D5C7FD-622A-40FA-828F-E3F2BF44ADE2}" name="Ciclo 2" dataDxfId="7"/>
+    <tableColumn id="16" xr3:uid="{11BFC6A6-81DE-4299-81B8-ACB7C83EFE82}" name="Ciclo 3" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{665865D4-79FD-48D9-9884-73E6CB75DCDC}" name="Observaciones" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{95C3BFB9-5AE9-4234-996A-372035075F8A}" name="Casos de prueba" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4402,7 +4694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7743D3-3A2E-4DC1-AE4F-246E9A34B1E2}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -4418,74 +4710,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>14</v>
+      <c r="A1" s="21" t="s">
+        <v>13</v>
       </c>
       <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="28">
+      <c r="B13">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="28">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="28">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="28">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="28">
+      <c r="B23">
         <v>8</v>
       </c>
     </row>
@@ -4499,8 +4791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2FD5888-1668-49CB-AEE5-B64C283366B2}">
   <dimension ref="B2:M40"/>
   <sheetViews>
-    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4517,282 +4809,285 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="12"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="31" t="s">
+      <c r="B2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
     </row>
     <row r="3" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="14"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
     </row>
     <row r="4" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="14"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="36"/>
-      <c r="F4" s="33" t="s">
+      <c r="B4" s="28"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="25"/>
+      <c r="F4" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+    </row>
+    <row r="5" spans="2:13" s="17" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="M5" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="10">
+        <v>1</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-    </row>
-    <row r="5" spans="2:13" s="23" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="25" t="s">
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="48" t="str">
+        <f t="shared" ref="H6:H13" si="0">HYPERLINK("#'Evidencias'!B4", "Evidencia")</f>
+        <v>Evidencia</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" s="8"/>
+      <c r="M6" s="11"/>
+    </row>
+    <row r="7" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="10">
+        <v>2</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="7"/>
+      <c r="M7" s="11"/>
+    </row>
+    <row r="8" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="10">
         <v>3</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="C8" s="9"/>
+      <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" s="8"/>
+      <c r="M8" s="11"/>
+    </row>
+    <row r="9" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="10">
         <v>4</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="C9" s="9"/>
+      <c r="D9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="8"/>
+      <c r="M9" s="11"/>
+    </row>
+    <row r="10" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="10">
         <v>5</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="C10" s="9"/>
+      <c r="D10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="8"/>
+      <c r="M10" s="11"/>
+    </row>
+    <row r="11" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="10">
         <v>6</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="C11" s="9"/>
+      <c r="D11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11" s="8"/>
+      <c r="M11" s="11"/>
+    </row>
+    <row r="12" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="12">
         <v>7</v>
       </c>
-      <c r="H5" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="M5" s="25" t="s">
+      <c r="C12" s="13"/>
+      <c r="D12" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="L12" s="15"/>
+      <c r="M12" s="16"/>
+    </row>
+    <row r="13" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="12">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="11">
-        <v>1</v>
-      </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="3" t="s">
+      <c r="C13" s="13"/>
+      <c r="D13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="L6" s="9"/>
-      <c r="M6" s="16"/>
-    </row>
-    <row r="7" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="11">
-        <v>2</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="3" t="s">
+      <c r="J13" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="K7" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="L7" s="8"/>
-      <c r="M7" s="16"/>
-    </row>
-    <row r="8" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="11">
-        <v>3</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="3" t="s">
+      <c r="K13" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="K8" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="L8" s="9"/>
-      <c r="M8" s="16"/>
-    </row>
-    <row r="9" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="11">
-        <v>4</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="K9" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="L9" s="9"/>
-      <c r="M9" s="16"/>
-    </row>
-    <row r="10" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="11">
-        <v>5</v>
-      </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="K10" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="L10" s="9"/>
-      <c r="M10" s="16"/>
-    </row>
-    <row r="11" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="11">
-        <v>6</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="J11" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="K11" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="L11" s="9"/>
-      <c r="M11" s="16"/>
-    </row>
-    <row r="12" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="17">
-        <v>7</v>
-      </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="J12" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="K12" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="L12" s="21"/>
-      <c r="M12" s="22"/>
-    </row>
-    <row r="13" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="17">
-        <v>8</v>
-      </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="J13" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="K13" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="L13" s="21"/>
-      <c r="M13" s="22"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="16"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F14" s="4"/>
@@ -4926,18 +5221,18 @@
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:C4"/>
-    <mergeCell ref="D2:M3"/>
     <mergeCell ref="F4:M4"/>
+    <mergeCell ref="F2:M3"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="I6:K13">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"Pendiente"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>"No aprobado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
       <formula>"Aprobado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4955,4 +5250,143 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828410E3-7509-432A-927E-46FE35382105}">
+  <dimension ref="A1:L7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:L4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="34"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="37"/>
+    </row>
+    <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="40"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="43"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="36">
+        <v>1</v>
+      </c>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="36">
+        <v>2</v>
+      </c>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="36">
+        <v>3</v>
+      </c>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="36">
+        <v>4</v>
+      </c>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="44"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B7:L7"/>
+    <mergeCell ref="C1:L1"/>
+    <mergeCell ref="C2:L2"/>
+    <mergeCell ref="B3:L3"/>
+    <mergeCell ref="B4:L4"/>
+    <mergeCell ref="B5:L5"/>
+    <mergeCell ref="B6:L6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>